<commit_message>
Se ha actualizado el contenido blanca
</commit_message>
<xml_diff>
--- a/B1-Blanca-Analisis de les propietats dels papers/practicas_laboratorio/Practica_1.xlsx
+++ b/B1-Blanca-Analisis de les propietats dels papers/practicas_laboratorio/Practica_1.xlsx
@@ -5,21 +5,25 @@
   <sheets>
     <sheet state="visible" name="gramatge y espesor" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Espesor Total" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Densidad" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="YVJdrIqE0qJTYAnrqKQyU1rkF6Ls4EI/810SFXnBILE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="SKy2OFALGdr9GyC5WIkP6qbHqENvvEaDqaAF+P9i4xs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>gramage</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Masa</t>
+  </si>
+  <si>
+    <t>Gramage</t>
   </si>
   <si>
     <t>espesor 1</t>
@@ -31,7 +35,16 @@
     <t>espesor 3</t>
   </si>
   <si>
-    <t>espesor Total</t>
+    <t>espesor de paquete</t>
+  </si>
+  <si>
+    <t>Espesor individual de paquete</t>
+  </si>
+  <si>
+    <t>Densidad individual</t>
+  </si>
+  <si>
+    <t>Densidad individal de paquete</t>
   </si>
 </sst>
 </file>
@@ -65,13 +78,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -85,6 +99,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -305,18 +323,25 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1.904</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
+        <f t="shared" ref="B2:B6" si="1">A2/0.01</f>
+        <v>190.4</v>
+      </c>
+      <c r="C2" s="1">
         <v>261.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>272.0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>258.0</v>
       </c>
     </row>
@@ -324,13 +349,17 @@
       <c r="A3" s="1">
         <v>1.877</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
+        <f t="shared" si="1"/>
+        <v>187.7</v>
+      </c>
+      <c r="C3" s="1">
         <v>259.0</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>257.0</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>256.0</v>
       </c>
     </row>
@@ -338,13 +367,17 @@
       <c r="A4" s="1">
         <v>1.855</v>
       </c>
-      <c r="B4" s="1">
-        <v>253.0</v>
+      <c r="B4" s="2">
+        <f t="shared" si="1"/>
+        <v>185.5</v>
       </c>
       <c r="C4" s="1">
         <v>253.0</v>
       </c>
       <c r="D4" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="E4" s="1">
         <v>258.0</v>
       </c>
     </row>
@@ -352,13 +385,17 @@
       <c r="A5" s="1">
         <v>1.873</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
+        <f t="shared" si="1"/>
+        <v>187.3</v>
+      </c>
+      <c r="C5" s="1">
         <v>264.0</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>257.0</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>253.0</v>
       </c>
     </row>
@@ -366,13 +403,17 @@
       <c r="A6" s="1">
         <v>1.825</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
+        <f t="shared" si="1"/>
+        <v>182.5</v>
+      </c>
+      <c r="C6" s="1">
         <v>252.0</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>254.0</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>249.0</v>
       </c>
     </row>
@@ -393,22 +434,100 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>1284.0</v>
       </c>
+      <c r="B2" s="2">
+        <f t="shared" ref="B2:B4" si="1">A2/5</f>
+        <v>256.8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
         <v>1278.0</v>
       </c>
+      <c r="B3" s="2">
+        <f t="shared" si="1"/>
+        <v>255.6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
         <v>1289.0</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="1"/>
+        <v>257.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <f>'gramatge y espesor'!B2/AVERAGE('gramatge y espesor'!C2:E2)</f>
+        <v>0.7221238938</v>
+      </c>
+      <c r="B2" s="2">
+        <f>'gramatge y espesor'!B2/AVERAGE('Espesor Total'!$B$2:$B$4)</f>
+        <v>0.7416255518</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <f>'gramatge y espesor'!B3/AVERAGE('gramatge y espesor'!C3:E3)</f>
+        <v>0.7294041451</v>
+      </c>
+      <c r="B3" s="2">
+        <f>'gramatge y espesor'!B3/AVERAGE('Espesor Total'!$B$2:$B$4)</f>
+        <v>0.7311088029</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <f>'gramatge y espesor'!B4/AVERAGE('gramatge y espesor'!C4:E4)</f>
+        <v>0.7284031414</v>
+      </c>
+      <c r="B4" s="2">
+        <f>'gramatge y espesor'!B4/AVERAGE('Espesor Total'!$B$2:$B$4)</f>
+        <v>0.7225396001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <f>'gramatge y espesor'!B5/AVERAGE('gramatge y espesor'!C5:E5)</f>
+        <v>0.7259689922</v>
+      </c>
+      <c r="B5" s="2">
+        <f>'gramatge y espesor'!B5/AVERAGE('Espesor Total'!$B$2:$B$4)</f>
+        <v>0.729550766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se ha actualizado la parte de blanca
</commit_message>
<xml_diff>
--- a/B1-Blanca-Analisis de les propietats dels papers/practicas_laboratorio/Practica_1.xlsx
+++ b/B1-Blanca-Analisis de les propietats dels papers/practicas_laboratorio/Practica_1.xlsx
@@ -20,31 +20,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Masa</t>
-  </si>
-  <si>
-    <t>Gramage</t>
-  </si>
-  <si>
-    <t>espesor 1</t>
-  </si>
-  <si>
-    <t>espesor 2</t>
-  </si>
-  <si>
-    <t>espesor 3</t>
-  </si>
-  <si>
-    <t>espesor de paquete</t>
-  </si>
-  <si>
-    <t>Espesor individual de paquete</t>
-  </si>
-  <si>
-    <t>Densidad individual</t>
-  </si>
-  <si>
-    <t>Densidad individal de paquete</t>
+    <t>Masa [$ g $]</t>
+  </si>
+  <si>
+    <t>Gramage [$ \frac(g){m^2} $</t>
+  </si>
+  <si>
+    <t>espesor [$ µm $] 1</t>
+  </si>
+  <si>
+    <t>espesor [$ µm $] 2</t>
+  </si>
+  <si>
+    <t>espesor [$ µm $] 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">espesor de paquete [$ µm $] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Espesor individual de paquete  [$ µm $] </t>
+  </si>
+  <si>
+    <t>Densidad individual [$ \frac{g}{cm^3} $]</t>
+  </si>
+  <si>
+    <t>Densidad individal de paquete [$ \frac{g}{cm^3} $]</t>
   </si>
 </sst>
 </file>

</xml_diff>